<commit_message>
added president's name to all approval excel files
</commit_message>
<xml_diff>
--- a/Input/bush_senior_approval.xlsx
+++ b/Input/bush_senior_approval.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="7">
   <si>
     <t>start_date_bush_senior</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>unsure_bush_senior</t>
+  </si>
+  <si>
+    <t>president</t>
+  </si>
+  <si>
+    <t>Bush, sr</t>
   </si>
 </sst>
 </file>
@@ -390,13 +396,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +418,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>33977</v>
       </c>
@@ -429,8 +438,11 @@
       <c r="E2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>33956</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="E3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>33942</v>
       </c>
@@ -463,8 +478,11 @@
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>33928</v>
       </c>
@@ -480,8 +498,11 @@
       <c r="E5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>33928</v>
       </c>
@@ -497,8 +518,11 @@
       <c r="E6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>33899</v>
       </c>
@@ -514,8 +538,11 @@
       <c r="E7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>33889</v>
       </c>
@@ -531,8 +558,11 @@
       <c r="E8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>33871</v>
       </c>
@@ -548,8 +578,11 @@
       <c r="E9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>33878</v>
       </c>
@@ -565,8 +598,11 @@
       <c r="E10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>33864</v>
       </c>
@@ -582,8 +618,11 @@
       <c r="E11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>33858</v>
       </c>
@@ -599,8 +638,11 @@
       <c r="E12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>33857</v>
       </c>
@@ -616,8 +658,11 @@
       <c r="E13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>33847</v>
       </c>
@@ -633,8 +678,11 @@
       <c r="E14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>33837</v>
       </c>
@@ -650,8 +698,11 @@
       <c r="E15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>33837</v>
       </c>
@@ -667,8 +718,11 @@
       <c r="E16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>33829</v>
       </c>
@@ -684,8 +738,11 @@
       <c r="E17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>33826</v>
       </c>
@@ -701,8 +758,11 @@
       <c r="E18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>33822</v>
       </c>
@@ -718,8 +778,11 @@
       <c r="E19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>33816</v>
       </c>
@@ -735,8 +798,11 @@
       <c r="E20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>33809</v>
       </c>
@@ -752,8 +818,11 @@
       <c r="E21">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>33808</v>
       </c>
@@ -769,8 +838,11 @@
       <c r="E22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>33781</v>
       </c>
@@ -786,8 +858,11 @@
       <c r="E23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>33767</v>
       </c>
@@ -803,8 +878,11 @@
       <c r="E24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>33759</v>
       </c>
@@ -820,8 +898,11 @@
       <c r="E25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>33742</v>
       </c>
@@ -837,8 +918,11 @@
       <c r="E26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>33717</v>
       </c>
@@ -854,8 +938,11 @@
       <c r="E27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>33731</v>
       </c>
@@ -871,8 +958,11 @@
       <c r="E28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>33714</v>
       </c>
@@ -888,8 +978,11 @@
       <c r="E29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>33703</v>
       </c>
@@ -905,8 +998,11 @@
       <c r="E30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>33689</v>
       </c>
@@ -922,8 +1018,11 @@
       <c r="E31">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>33675</v>
       </c>
@@ -939,8 +1038,11 @@
       <c r="E32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
         <v>33683</v>
       </c>
@@ -956,8 +1058,11 @@
       <c r="E33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>33674</v>
       </c>
@@ -973,8 +1078,11 @@
       <c r="E34">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
         <v>33662</v>
       </c>
@@ -990,8 +1098,11 @@
       <c r="E35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>33648</v>
       </c>
@@ -1007,8 +1118,11 @@
       <c r="E36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
         <v>33654</v>
       </c>
@@ -1024,8 +1138,11 @@
       <c r="E37">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
         <v>33653</v>
       </c>
@@ -1041,8 +1158,11 @@
       <c r="E38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
         <v>33640</v>
       </c>
@@ -1058,8 +1178,11 @@
       <c r="E39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
         <v>33634</v>
       </c>
@@ -1075,8 +1198,11 @@
       <c r="E40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
         <v>33631</v>
       </c>
@@ -1092,8 +1218,11 @@
       <c r="E41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
         <v>33619</v>
       </c>
@@ -1109,8 +1238,11 @@
       <c r="E42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
         <v>33606</v>
       </c>
@@ -1126,8 +1258,11 @@
       <c r="E43">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>33563</v>
       </c>
@@ -1143,8 +1278,11 @@
       <c r="E44">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>33535</v>
       </c>
@@ -1160,8 +1298,11 @@
       <c r="E45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
         <v>33528</v>
       </c>
@@ -1177,8 +1318,11 @@
       <c r="E46">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
         <v>33521</v>
       </c>
@@ -1194,8 +1338,11 @@
       <c r="E47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
         <v>33482</v>
       </c>
@@ -1211,8 +1358,11 @@
       <c r="E48">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
         <v>33507</v>
       </c>
@@ -1228,8 +1378,11 @@
       <c r="E49">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
         <v>33491</v>
       </c>
@@ -1245,8 +1398,11 @@
       <c r="E50">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
         <v>33479</v>
       </c>
@@ -1262,8 +1418,11 @@
       <c r="E51">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
         <v>33451</v>
       </c>
@@ -1279,8 +1438,11 @@
       <c r="E52">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
         <v>33473</v>
       </c>
@@ -1296,8 +1458,11 @@
       <c r="E53">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
         <v>33458</v>
       </c>
@@ -1313,8 +1478,11 @@
       <c r="E54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
         <v>33458</v>
       </c>
@@ -1330,8 +1498,11 @@
       <c r="E55">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
         <v>33444</v>
       </c>
@@ -1347,8 +1518,11 @@
       <c r="E56">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
         <v>33426</v>
       </c>
@@ -1364,8 +1538,11 @@
       <c r="E57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
         <v>33437</v>
       </c>
@@ -1381,8 +1558,11 @@
       <c r="E58">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
         <v>33430</v>
       </c>
@@ -1398,8 +1578,11 @@
       <c r="E59">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
         <v>33415</v>
       </c>
@@ -1415,8 +1598,11 @@
       <c r="E60">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
         <v>33395</v>
       </c>
@@ -1432,8 +1618,11 @@
       <c r="E61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
         <v>33402</v>
       </c>
@@ -1449,8 +1638,11 @@
       <c r="E62">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
         <v>33388</v>
       </c>
@@ -1466,8 +1658,11 @@
       <c r="E63">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
         <v>33381</v>
       </c>
@@ -1483,8 +1678,11 @@
       <c r="E64">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="2">
         <v>33374</v>
       </c>
@@ -1500,8 +1698,11 @@
       <c r="E65">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="2">
         <v>33360</v>
       </c>
@@ -1517,8 +1718,11 @@
       <c r="E66">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="2">
         <v>33353</v>
       </c>
@@ -1534,8 +1738,11 @@
       <c r="E67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="2">
         <v>33351</v>
       </c>
@@ -1551,8 +1758,11 @@
       <c r="E68">
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="2">
         <v>33339</v>
       </c>
@@ -1568,8 +1778,11 @@
       <c r="E69">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="2">
         <v>33332</v>
       </c>
@@ -1585,8 +1798,11 @@
       <c r="E70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="2">
         <v>33325</v>
       </c>
@@ -1602,8 +1818,11 @@
       <c r="E71">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="2">
         <v>33318</v>
       </c>
@@ -1619,8 +1838,11 @@
       <c r="E72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="2">
         <v>33311</v>
       </c>
@@ -1636,8 +1858,11 @@
       <c r="E73">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="2">
         <v>33304</v>
       </c>
@@ -1653,8 +1878,11 @@
       <c r="E74">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="2">
         <v>33285</v>
       </c>
@@ -1670,8 +1898,11 @@
       <c r="E75">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="2">
         <v>33297</v>
       </c>
@@ -1687,8 +1918,11 @@
       <c r="E76">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="2">
         <v>33290</v>
       </c>
@@ -1704,8 +1938,11 @@
       <c r="E77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" s="2">
         <v>33283</v>
       </c>
@@ -1721,8 +1958,11 @@
       <c r="E78">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="2">
         <v>33283</v>
       </c>
@@ -1738,8 +1978,11 @@
       <c r="E79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" s="2">
         <v>33276</v>
       </c>
@@ -1755,8 +1998,11 @@
       <c r="E80">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="2">
         <v>33264</v>
       </c>
@@ -1772,8 +2018,11 @@
       <c r="E81">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="2">
         <v>33261</v>
       </c>
@@ -1789,8 +2038,11 @@
       <c r="E82">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="2">
         <v>33262</v>
       </c>
@@ -1806,8 +2058,11 @@
       <c r="E83">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="2">
         <v>33257</v>
       </c>
@@ -1823,8 +2078,11 @@
       <c r="E84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="2">
         <v>33255</v>
       </c>
@@ -1840,8 +2098,11 @@
       <c r="E85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="2">
         <v>33255</v>
       </c>
@@ -1857,8 +2118,11 @@
       <c r="E86">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="2">
         <v>33249</v>
       </c>
@@ -1874,8 +2138,11 @@
       <c r="E87">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="2">
         <v>33248</v>
       </c>
@@ -1891,8 +2158,11 @@
       <c r="E88">
         <v>9</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="2">
         <v>33241</v>
       </c>
@@ -1908,8 +2178,11 @@
       <c r="E89">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="2">
         <v>33214</v>
       </c>
@@ -1925,8 +2198,11 @@
       <c r="E90">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="2">
         <v>33220</v>
       </c>
@@ -1942,8 +2218,11 @@
       <c r="E91">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="2">
         <v>33213</v>
       </c>
@@ -1959,8 +2238,11 @@
       <c r="E92">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="2">
         <v>33213</v>
       </c>
@@ -1976,8 +2258,11 @@
       <c r="E93">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="2">
         <v>33206</v>
       </c>
@@ -1993,8 +2278,11 @@
       <c r="E94">
         <v>10</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="2">
         <v>33186</v>
       </c>
@@ -2010,8 +2298,11 @@
       <c r="E95">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="2">
         <v>33192</v>
       </c>
@@ -2027,8 +2318,11 @@
       <c r="E96">
         <v>13</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="2">
         <v>33192</v>
       </c>
@@ -2044,8 +2338,11 @@
       <c r="E97">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="2">
         <v>33185</v>
       </c>
@@ -2061,8 +2358,11 @@
       <c r="E98">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="2">
         <v>33171</v>
       </c>
@@ -2078,8 +2378,11 @@
       <c r="E99">
         <v>10</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="2">
         <v>33164</v>
       </c>
@@ -2095,8 +2398,11 @@
       <c r="E100">
         <v>10</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="2">
         <v>33164</v>
       </c>
@@ -2112,8 +2418,11 @@
       <c r="E101">
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="2">
         <v>33157</v>
       </c>
@@ -2129,8 +2438,11 @@
       <c r="E102">
         <v>10</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="2">
         <v>33137</v>
       </c>
@@ -2146,8 +2458,11 @@
       <c r="E103">
         <v>11</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="2">
         <v>33149</v>
       </c>
@@ -2163,8 +2478,11 @@
       <c r="E104">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" s="2">
         <v>33143</v>
       </c>
@@ -2180,8 +2498,11 @@
       <c r="E105">
         <v>12</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" s="2">
         <v>33130</v>
       </c>
@@ -2197,8 +2518,11 @@
       <c r="E106">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="2">
         <v>33127</v>
       </c>
@@ -2214,8 +2538,11 @@
       <c r="E107">
         <v>11</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" s="2">
         <v>33126</v>
       </c>
@@ -2231,8 +2558,11 @@
       <c r="E108">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" s="2">
         <v>33115</v>
       </c>
@@ -2248,8 +2578,11 @@
       <c r="E109">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" s="2">
         <v>33095</v>
       </c>
@@ -2265,8 +2598,11 @@
       <c r="E110">
         <v>11</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="2">
         <v>33108</v>
       </c>
@@ -2282,8 +2618,11 @@
       <c r="E111">
         <v>7</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="2">
         <v>33108</v>
       </c>
@@ -2299,8 +2638,11 @@
       <c r="E112">
         <v>10</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" s="2">
         <v>33101</v>
       </c>
@@ -2316,8 +2658,11 @@
       <c r="E113">
         <v>8</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" s="2">
         <v>33094</v>
       </c>
@@ -2333,8 +2678,11 @@
       <c r="E114">
         <v>10</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" s="2">
         <v>33074</v>
       </c>
@@ -2350,8 +2698,11 @@
       <c r="E115">
         <v>12</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" s="2">
         <v>33094</v>
       </c>
@@ -2367,8 +2718,11 @@
       <c r="E116">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" s="2">
         <v>33073</v>
       </c>
@@ -2384,8 +2738,11 @@
       <c r="E117">
         <v>14</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" s="2">
         <v>33061</v>
       </c>
@@ -2401,8 +2758,11 @@
       <c r="E118">
         <v>15</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" s="2">
         <v>33066</v>
       </c>
@@ -2418,8 +2778,11 @@
       <c r="E119">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="2">
         <v>33059</v>
       </c>
@@ -2435,8 +2798,11 @@
       <c r="E120">
         <v>12</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" s="2">
         <v>33038</v>
       </c>
@@ -2452,8 +2818,11 @@
       <c r="E121">
         <v>14</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" s="2">
         <v>32997</v>
       </c>
@@ -2469,8 +2838,11 @@
       <c r="E122">
         <v>13</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="2">
         <v>32997</v>
       </c>
@@ -2486,8 +2858,11 @@
       <c r="E123">
         <v>13</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" s="2">
         <v>32969</v>
       </c>
@@ -2503,8 +2878,11 @@
       <c r="E124">
         <v>13</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" s="2">
         <v>32968</v>
       </c>
@@ -2520,8 +2898,11 @@
       <c r="E125">
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" s="2">
         <v>32948</v>
       </c>
@@ -2537,8 +2918,11 @@
       <c r="E126">
         <v>8</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" s="2">
         <v>32940</v>
       </c>
@@ -2554,8 +2938,11 @@
       <c r="E127">
         <v>13</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" s="2">
         <v>32913</v>
       </c>
@@ -2571,8 +2958,11 @@
       <c r="E128">
         <v>11</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" s="2">
         <v>32919</v>
       </c>
@@ -2588,8 +2978,11 @@
       <c r="E129">
         <v>11</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" s="2">
         <v>32912</v>
       </c>
@@ -2605,8 +2998,11 @@
       <c r="E130">
         <v>10</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" s="2">
         <v>32850</v>
       </c>
@@ -2622,8 +3018,11 @@
       <c r="E131">
         <v>17</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" s="2">
         <v>32877</v>
       </c>
@@ -2639,8 +3038,11 @@
       <c r="E132">
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" s="2">
         <v>32849</v>
       </c>
@@ -2656,8 +3058,11 @@
       <c r="E133">
         <v>8</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="2">
         <v>32822</v>
       </c>
@@ -2673,8 +3078,11 @@
       <c r="E134">
         <v>14</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" s="2">
         <v>32821</v>
       </c>
@@ -2690,8 +3098,11 @@
       <c r="E135">
         <v>13</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" s="2">
         <v>32794</v>
       </c>
@@ -2707,8 +3118,11 @@
       <c r="E136">
         <v>17</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" s="2">
         <v>32786</v>
       </c>
@@ -2724,8 +3138,11 @@
       <c r="E137">
         <v>12</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" s="2">
         <v>32786</v>
       </c>
@@ -2741,8 +3158,11 @@
       <c r="E138">
         <v>15</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="2">
         <v>32773</v>
       </c>
@@ -2758,8 +3178,11 @@
       <c r="E139">
         <v>14</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" s="2">
         <v>32758</v>
       </c>
@@ -2775,8 +3198,11 @@
       <c r="E140">
         <v>13</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" s="2">
         <v>32735</v>
       </c>
@@ -2792,8 +3218,11 @@
       <c r="E141">
         <v>17</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" s="2">
         <v>32728</v>
       </c>
@@ -2809,8 +3238,11 @@
       <c r="E142">
         <v>19</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" s="2">
         <v>32730</v>
       </c>
@@ -2826,8 +3258,11 @@
       <c r="E143">
         <v>12</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" s="2">
         <v>32695</v>
       </c>
@@ -2843,8 +3278,11 @@
       <c r="E144">
         <v>15</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="2">
         <v>32668</v>
       </c>
@@ -2860,8 +3298,11 @@
       <c r="E145">
         <v>20</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="2">
         <v>32667</v>
       </c>
@@ -2877,8 +3318,11 @@
       <c r="E146">
         <v>16</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="2">
         <v>32660</v>
       </c>
@@ -2894,8 +3338,11 @@
       <c r="E147">
         <v>19</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" s="2">
         <v>32643</v>
       </c>
@@ -2911,8 +3358,11 @@
       <c r="E148">
         <v>19</v>
       </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="F148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" s="2">
         <v>32640</v>
       </c>
@@ -2928,8 +3378,11 @@
       <c r="E149">
         <v>16</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" s="2">
         <v>32633</v>
       </c>
@@ -2945,8 +3398,11 @@
       <c r="E150">
         <v>23</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" s="2">
         <v>32632</v>
       </c>
@@ -2962,8 +3418,11 @@
       <c r="E151">
         <v>22</v>
       </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="F151" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" s="2">
         <v>32633</v>
       </c>
@@ -2979,8 +3438,11 @@
       <c r="E152">
         <v>20</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153" s="2">
         <v>32608</v>
       </c>
@@ -2996,8 +3458,11 @@
       <c r="E153">
         <v>26</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" s="2">
         <v>32605</v>
       </c>
@@ -3013,8 +3478,11 @@
       <c r="E154">
         <v>27</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" s="2">
         <v>32577</v>
       </c>
@@ -3030,8 +3498,11 @@
       <c r="E155">
         <v>27</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" s="2">
         <v>32576</v>
       </c>
@@ -3047,8 +3518,11 @@
       <c r="E156">
         <v>22</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" s="2">
         <v>32567</v>
       </c>
@@ -3064,8 +3538,11 @@
       <c r="E157">
         <v>24</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" s="2">
         <v>32563</v>
       </c>
@@ -3081,8 +3558,11 @@
       <c r="E158">
         <v>27</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="F158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159" s="2">
         <v>32532</v>
       </c>
@@ -3097,6 +3577,9 @@
       </c>
       <c r="E159">
         <v>43</v>
+      </c>
+      <c r="F159" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>